<commit_message>
Test Data Comment column updated for login and reset password
</commit_message>
<xml_diff>
--- a/DataSet/TestData.xlsx
+++ b/DataSet/TestData.xlsx
@@ -3,12 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26731"/>
   <workbookPr defaultThemeVersion="166925"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\pinky\Selenium\LMSAutomation\DataSet\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{59692964-44DB-4763-8E9F-8D953CDBC2A1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:801_{49FD9F65-CF31-4184-9C07-0CD710190B86}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="1" xr2:uid="{0D3C3A0C-7FA1-413F-8B14-49114F2CD0BF}"/>
   </bookViews>
@@ -16,7 +11,8 @@
     <sheet name="Login_Page" sheetId="1" r:id="rId1"/>
     <sheet name="Reset_Password" sheetId="2" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="191029"/>
+  <calcPr calcId="0"/>
+  <oleSize ref="A1:P24"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -37,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="12">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="33" uniqueCount="26">
   <si>
     <t>UserName</t>
   </si>
@@ -73,13 +69,55 @@
   </si>
   <si>
     <t>Abc!12</t>
+  </si>
+  <si>
+    <t>Comment</t>
+  </si>
+  <si>
+    <t>Valid Credential</t>
+  </si>
+  <si>
+    <t>Invalid Credentials</t>
+  </si>
+  <si>
+    <t>Blank User Name,Valid Passwprd</t>
+  </si>
+  <si>
+    <t>Valid User name , Blank Password</t>
+  </si>
+  <si>
+    <t>sdffsdsd</t>
+  </si>
+  <si>
+    <t>Valid Username,Invalid pw</t>
+  </si>
+  <si>
+    <t>dfdssss</t>
+  </si>
+  <si>
+    <t>InValid Username,Valid pw</t>
+  </si>
+  <si>
+    <t>Empty User name and password</t>
+  </si>
+  <si>
+    <t>Valid details</t>
+  </si>
+  <si>
+    <t>Invalid details</t>
+  </si>
+  <si>
+    <t>Empty details</t>
+  </si>
+  <si>
+    <t>Mismatch values</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -103,6 +141,12 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FF000000"/>
+      <name val="Consolas"/>
+      <family val="3"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -125,10 +169,13 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -444,50 +491,93 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9F097C1D-6250-4702-8B35-4D6D98A8C00D}">
-  <dimension ref="A1:B5"/>
+  <dimension ref="A1:C8"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A8" sqref="A8"/>
+      <selection activeCell="C18" sqref="C18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="15.21875" customWidth="1"/>
     <col min="2" max="2" width="13.44140625" customWidth="1"/>
+    <col min="3" max="3" width="31.5546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:3" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
         <v>1</v>
       </c>
-    </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C1" s="1" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>4</v>
       </c>
       <c r="B2" s="2" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C2" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>2</v>
       </c>
       <c r="B3" s="2" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C3" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
       <c r="B4" s="2" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C4" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>4</v>
+      </c>
+      <c r="C5" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A6" t="s">
+        <v>4</v>
+      </c>
+      <c r="B6" t="s">
+        <v>17</v>
+      </c>
+      <c r="C6" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A7" t="s">
+        <v>19</v>
+      </c>
+      <c r="B7" t="s">
+        <v>3</v>
+      </c>
+      <c r="C7" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="C8" t="s">
+        <v>21</v>
       </c>
     </row>
   </sheetData>
@@ -503,48 +593,66 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0F105EE8-F943-4097-A021-78D6133EDBB8}">
-  <dimension ref="A1:B5"/>
+  <dimension ref="A1:C5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E16" sqref="E16"/>
+      <selection activeCell="C16" sqref="C16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="15.33203125" customWidth="1"/>
     <col min="2" max="2" width="14.5546875" customWidth="1"/>
+    <col min="3" max="3" width="25" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A1" t="s">
+    <row r="1" spans="1:3" s="1" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A1" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="B1" t="s">
+      <c r="B1" s="1" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C1" s="1" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A2" s="2" t="s">
         <v>8</v>
       </c>
       <c r="B2" s="2" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C2" s="3" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>9</v>
       </c>
       <c r="B3" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C3" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="C4" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>10</v>
       </c>
       <c r="B5" t="s">
         <v>11</v>
+      </c>
+      <c r="C5" t="s">
+        <v>25</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
program and batch modules are done
</commit_message>
<xml_diff>
--- a/DataSet/TestData.xlsx
+++ b/DataSet/TestData.xlsx
@@ -8,14 +8,15 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\priya\eclipse-workspace\LMSAutomation\DataSet\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E1F408E9-2325-480D-B5CC-95C2EF328329}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C50CFC8C-9F1E-444C-8E3F-55951A924F16}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11040" activeTab="2" xr2:uid="{0D3C3A0C-7FA1-413F-8B14-49114F2CD0BF}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11040" activeTab="3" xr2:uid="{0D3C3A0C-7FA1-413F-8B14-49114F2CD0BF}"/>
   </bookViews>
   <sheets>
     <sheet name="Login_Page" sheetId="1" r:id="rId1"/>
     <sheet name="Reset_Password" sheetId="2" r:id="rId2"/>
     <sheet name="program" sheetId="3" r:id="rId3"/>
+    <sheet name="batch" sheetId="4" r:id="rId4"/>
   </sheets>
   <calcPr calcId="0"/>
   <extLst>
@@ -27,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="43" uniqueCount="35">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="58" uniqueCount="49">
   <si>
     <t>UserName</t>
   </si>
@@ -132,6 +133,48 @@
   </si>
   <si>
     <t>Bootcamp</t>
+  </si>
+  <si>
+    <t>sdet115_2023</t>
+  </si>
+  <si>
+    <t>batchname</t>
+  </si>
+  <si>
+    <t>batchdescription</t>
+  </si>
+  <si>
+    <t>noofclasses</t>
+  </si>
+  <si>
+    <t>sdet116_2023</t>
+  </si>
+  <si>
+    <t>DA</t>
+  </si>
+  <si>
+    <t>abc$</t>
+  </si>
+  <si>
+    <t>salesforce</t>
+  </si>
+  <si>
+    <t>Sdet_117</t>
+  </si>
+  <si>
+    <t>TESTING</t>
+  </si>
+  <si>
+    <t>abc</t>
+  </si>
+  <si>
+    <t>def</t>
+  </si>
+  <si>
+    <t>hn</t>
+  </si>
+  <si>
+    <t>Sdet_118</t>
   </si>
 </sst>
 </file>
@@ -689,8 +732,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{40813197-443F-41B1-A446-15E71DAF58B9}">
   <dimension ref="A1:B7"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A3" sqref="A3"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A8" sqref="A8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -747,4 +790,102 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{62EEB348-6315-4DC5-B32F-97F420BF2487}">
+  <dimension ref="A1:C10"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C10" sqref="C10"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="16.5703125" customWidth="1"/>
+    <col min="2" max="2" width="15.85546875" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>36</v>
+      </c>
+      <c r="B1" t="s">
+        <v>37</v>
+      </c>
+      <c r="C1" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>35</v>
+      </c>
+      <c r="C2">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>39</v>
+      </c>
+      <c r="B3" t="s">
+        <v>40</v>
+      </c>
+      <c r="C3">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>41</v>
+      </c>
+      <c r="B4" t="s">
+        <v>40</v>
+      </c>
+      <c r="C4">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B5" t="s">
+        <v>42</v>
+      </c>
+      <c r="C5">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>43</v>
+      </c>
+      <c r="B7" t="s">
+        <v>44</v>
+      </c>
+      <c r="C7">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>45</v>
+      </c>
+      <c r="B8" t="s">
+        <v>46</v>
+      </c>
+      <c r="C8" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>48</v>
+      </c>
+      <c r="C10">
+        <v>7</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>